<commit_message>
Made changes to comments.
</commit_message>
<xml_diff>
--- a/BodyMassIndex/Documents/Lab 2 - Desk Check.xlsx
+++ b/BodyMassIndex/Documents/Lab 2 - Desk Check.xlsx
@@ -498,19 +498,19 @@
       </c>
       <c r="B7">
         <f ca="1">RANDBETWEEN(80,300)</f>
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C7" s="1">
         <f ca="1">RANDBETWEEN(40,80)</f>
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ref="D7:D25" ca="1" si="0">ROUND(((B7/(C7^2))*703),1)</f>
-        <v>12.7</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="E7" s="4" t="str">
         <f t="shared" ref="E7:E25" ca="1" si="1">IF(D7&lt;$G$6,$H$6,IF(D7&lt;$G$7,$H$7,IF(D7&lt;$G$8,$H$8,IF(D7&lt;$G$9,$H$9,IF(D7&gt;=$G$10,$H$10,"Error")))))</f>
-        <v>severely underweight</v>
+        <v>obese</v>
       </c>
       <c r="G7" s="4">
         <v>18.5</v>
@@ -525,19 +525,19 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B25" ca="1" si="2">RANDBETWEEN(80,300)</f>
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" ref="C8:C25" ca="1" si="3">RANDBETWEEN(40,80)</f>
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>25.3</v>
+        <v>66.5</v>
       </c>
       <c r="E8" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>overweight</v>
+        <v>obese</v>
       </c>
       <c r="G8" s="4">
         <v>25</v>
@@ -552,7 +552,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="2"/>
-        <v>244</v>
+        <v>162</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" ca="1" si="3"/>
@@ -560,7 +560,7 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>84.7</v>
+        <v>56.2</v>
       </c>
       <c r="E9" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -579,19 +579,19 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="2"/>
-        <v>91</v>
+        <v>228</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>19.7</v>
+        <v>25.7</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>healthy</v>
+        <v>overweight</v>
       </c>
       <c r="G10" s="4">
         <v>30</v>
@@ -606,15 +606,15 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="2"/>
-        <v>220</v>
+        <v>249</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>51.1</v>
+        <v>47</v>
       </c>
       <c r="E11" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -627,15 +627,15 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="2"/>
-        <v>148</v>
+        <v>289</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>33.200000000000003</v>
+        <v>60.4</v>
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -648,19 +648,19 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="2"/>
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>52.1</v>
+        <v>25.4</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>obese</v>
+        <v>overweight</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -669,15 +669,15 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="2"/>
-        <v>281</v>
+        <v>111</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>30.9</v>
+        <v>44.2</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -690,15 +690,15 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="2"/>
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>45.7</v>
+        <v>63.8</v>
       </c>
       <c r="E15" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -711,15 +711,15 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="2"/>
-        <v>229</v>
+        <v>268</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>87.1</v>
+        <v>117.8</v>
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -732,15 +732,15 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="2"/>
-        <v>293</v>
+        <v>180</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>57.2</v>
+        <v>30</v>
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -753,15 +753,15 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="2"/>
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D18" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>78.099999999999994</v>
+        <v>71.900000000000006</v>
       </c>
       <c r="E18" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -774,15 +774,15 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="2"/>
-        <v>239</v>
+        <v>144</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>42.3</v>
+        <v>52.3</v>
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -795,19 +795,19 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <v>200</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>36.6</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>healthy</v>
+        <v>obese</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -816,15 +816,15 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <v>223</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>41</v>
+        <v>60</v>
       </c>
       <c r="D21" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>33.5</v>
+        <v>43.5</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -837,15 +837,15 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="2"/>
-        <v>263</v>
+        <v>99</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="D22" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>37.6</v>
       </c>
       <c r="E22" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -858,19 +858,19 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="2"/>
-        <v>185</v>
+        <v>262</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="D23" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>overweight</v>
+        <v>obese</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -879,19 +879,19 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="2"/>
-        <v>92</v>
+        <v>261</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>28.1</v>
+        <v>86.7</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>overweight</v>
+        <v>obese</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -900,19 +900,19 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="2"/>
-        <v>93</v>
+        <v>240</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D25" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>23.3</v>
+        <v>48.5</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>healthy</v>
+        <v>obese</v>
       </c>
     </row>
   </sheetData>

</xml_diff>